<commit_message>
more writer utils added
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/poiwriter.xlsx
+++ b/src/test/resources/XLSXFiles/poiwriter.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t/>
   </si>
   <si>
     <t>EA ONE</t>
+  </si>
+  <si>
+    <t>EA TWO</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -72,6 +75,9 @@
       <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="B1" t="s" s="0">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
added cell updator poi
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/poiwriter.xlsx
+++ b/src/test/resources/XLSXFiles/poiwriter.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t/>
   </si>
@@ -21,6 +21,18 @@
   </si>
   <si>
     <t>EA TWO</t>
+  </si>
+  <si>
+    <t>EA FIVE</t>
+  </si>
+  <si>
+    <t>EA THREE</t>
+  </si>
+  <si>
+    <t>EA FOUR</t>
+  </si>
+  <si>
+    <t>EA TEST</t>
   </si>
 </sst>
 </file>
@@ -65,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -78,6 +90,15 @@
       <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
added row and column wise updator
</commit_message>
<xml_diff>
--- a/src/test/resources/XLSXFiles/poiwriter.xlsx
+++ b/src/test/resources/XLSXFiles/poiwriter.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="7">
   <si>
     <t/>
   </si>
@@ -97,7 +97,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>